<commit_message>
Fix some errors and add more functions
</commit_message>
<xml_diff>
--- a/data/MutationHistogram.xlsx
+++ b/data/MutationHistogram.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumente\Programmierungen\workspace\DNA_Distribution_Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC722077-6D6C-47AC-948F-7CD205E1C8A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B43EC-BDA6-4B5C-90F0-16CD325D5631}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1" xr2:uid="{ED56AE05-34A8-4193-BE17-B6923726E001}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{ED56AE05-34A8-4193-BE17-B6923726E001}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Ohne Gewichtungen</t>
   </si>
@@ -58,9 +59,6 @@
   </si>
   <si>
     <t>Differenzhistogramm: Fehler bei keiner Gewichtung_x000B_gegenüber Fehler mit TA+TA+TT Gewichtung_x000B_(Natürlicher Code, CCDS Mensch)_x000B_Positiv: Mehr Fehler in diesem Bereich mit Gewichtungen</t>
-  </si>
-  <si>
-    <t>Ohne Gewichttungen</t>
   </si>
 </sst>
 </file>
@@ -211,13 +209,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ohne Gewichttungen</c:v>
+                  <c:v>Ohne Gewichtungen</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -879,7 +877,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1545,6 +1543,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Quadrat. Fehler</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1610,6 +1663,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anzahl Mutationen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1699,9 +1807,9 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="76200" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:srgbClr val="FF0000"/>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1742,194 +1850,20 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+            <a:pPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Differenz der Histogramme:</a:t>
+              <a:rPr lang="de-DE" sz="1400" b="0"/>
+              <a:t>Histogrammvergleich der Fehler mit und ohne Gewichtungen</a:t>
             </a:r>
-            <a:br>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-            </a:br>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Positiv: Mehr Werte mit Gewichtungen</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-            </a:br>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Negativ: Mehr Werte ohne Gewichtungen</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Unten: Histogramme alle Fehler die in den GMS Score einfließen mit</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-            </a:br>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>und ohne Gewichtungen (NA+TA+TT)</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.21594807397450896"/>
-          <c:y val="0.62018856817905588"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1948,1947 +1882,12 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$F$2:$F$103</c:f>
-              <c:strCache>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>und größer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$I$2:$I$103</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-67</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3523-450F-8F01-F7B00699C790}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$F$2:$F$103</c:f>
-              <c:strCache>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>und größer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$I$2:$I$103</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-67</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3523-450F-8F01-F7B00699C790}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$F$2:$F$103</c:f>
-              <c:strCache>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>und größer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$I$2:$I$103</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="102"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-67</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3523-450F-8F01-F7B00699C790}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="0"/>
           <c:order val="3"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4544,6 +2543,1987 @@
         <c:smooth val="0"/>
         <c:axId val="546343024"/>
         <c:axId val="546341384"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="0"/>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$F$2:$F$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>54</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>59</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>68</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>73</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>74</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>76</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>78</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>79</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>81</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>82</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>86</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>87</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>88</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>89</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>91</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>92</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>94</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>95</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>97</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>98</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>99</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>und größer</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$I$2:$I$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-67</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-15</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-12</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-9</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-13</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>-4</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>9</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-3523-450F-8F01-F7B00699C790}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$F$2:$F$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>54</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>59</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>68</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>73</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>74</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>76</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>78</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>79</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>81</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>82</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>86</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>87</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>88</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>89</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>91</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>92</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>94</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>95</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>97</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>98</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>99</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>und größer</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$I$2:$I$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-67</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-15</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-12</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-9</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-13</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>-4</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>9</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3523-450F-8F01-F7B00699C790}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="2"/>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$F$2:$F$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>54</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>57</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>58</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>59</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>61</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>62</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>68</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>69</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>71</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>73</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>74</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>75</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>76</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>78</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>79</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>80</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>81</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>82</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>83</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>86</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>87</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>88</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>89</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>91</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>92</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>93</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>94</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>95</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>96</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>97</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>98</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>99</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>und größer</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$I$2:$I$103</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="102"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-67</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-15</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-12</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-9</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>-11</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>-13</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>-1</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>-4</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>-3</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>-2</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>-5</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>9</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3523-450F-8F01-F7B00699C790}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="546343024"/>
@@ -4552,10 +4532,56 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Quadrat. Fehler</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46081966530601104"/>
+              <c:y val="0.84319106716442993"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4570,7 +4596,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4593,7 +4619,7 @@
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="0"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -4617,6 +4643,79 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Differenz Anzahl</a:t>
+                </a:r>
+                <a:br>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                </a:br>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t> Mutationen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.7424204582308072E-2"/>
+              <c:y val="0.55083023220386929"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4632,8 +4731,8 @@
           <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:pPr algn="ctr">
+              <a:defRPr lang="de-DE" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4650,8 +4749,13 @@
         </c:txPr>
         <c:crossAx val="546343024"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -4661,11 +4765,9 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="76200" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="accent1">
-          <a:lumMod val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -5250,15 +5352,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>657226</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>12246</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>336176</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>112940</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5287,16 +5389,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>593912</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>410766</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>10026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>336177</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>115304</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>60831</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5625,14 +5727,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070CF82B-0770-4F98-ADE4-24090298FE14}">
   <dimension ref="A1:M1174"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -5649,7 +5752,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>1</v>
@@ -16698,8 +16801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2735710-04A2-4BBA-B7FF-77D347C31ADE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A39" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add hydropathy as weight parameter
</commit_message>
<xml_diff>
--- a/data/MutationHistogram.xlsx
+++ b/data/MutationHistogram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumente\Programmierungen\workspace\DNA_Distribution_Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B43EC-BDA6-4B5C-90F0-16CD325D5631}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C771464-37E1-483B-A7C6-43BC3AC7906F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{ED56AE05-34A8-4193-BE17-B6923726E001}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{ED56AE05-34A8-4193-BE17-B6923726E001}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -3219,7 +3219,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$F$2:$F$103</c15:sqref>
@@ -3539,7 +3539,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$I$2:$I$103</c15:sqref>
@@ -3859,7 +3859,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-3523-450F-8F01-F7B00699C790}"/>
                   </c:ext>
@@ -3875,7 +3875,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$F$2:$F$103</c15:sqref>
@@ -4195,7 +4195,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$I$2:$I$103</c15:sqref>
@@ -4515,7 +4515,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-3523-450F-8F01-F7B00699C790}"/>
                   </c:ext>

</xml_diff>